<commit_message>
Update test to match changes in REST API v1.4
</commit_message>
<xml_diff>
--- a/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
+++ b/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
@@ -147,10 +147,10 @@
     <t>All breast cancer</t>
   </si>
   <si>
-    <t>1.53 [1.50, 1.56]</t>
-  </si>
-  <si>
-    <t>0.522 [0.519, 0.527]</t>
+    <t>1.53 [1.5,1.56]</t>
+  </si>
+  <si>
+    <t>0.522 [0.519,0.527]</t>
   </si>
   <si>
     <t>Number of Individuals</t>

</xml_diff>

<commit_message>
Add ancestry distribution data to the export files
</commit_message>
<xml_diff>
--- a/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
+++ b/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="93">
   <si>
     <t>Polygenic Score (PGS) ID</t>
   </si>
@@ -63,6 +63,15 @@
     <t>Score and results match the original publication</t>
   </si>
   <si>
+    <t>Ancestry Distribution (%) - Source of Variant Associations (GWAS)</t>
+  </si>
+  <si>
+    <t>Ancestry Distribution (%) - Score Development/Training</t>
+  </si>
+  <si>
+    <t>Ancestry Distribution (%) - PGS Evaluation</t>
+  </si>
+  <si>
     <t>FTP link</t>
   </si>
   <si>
@@ -99,6 +108,15 @@
     <t>10.1010/test/test1</t>
   </si>
   <si>
+    <t>Multi-ancestry (including European):100</t>
+  </si>
+  <si>
+    <t>European:100</t>
+  </si>
+  <si>
+    <t>European:66.7|Multi-ancestry (including European):33.3</t>
+  </si>
+  <si>
     <t>http://ftp.ebi.ac.uk/pub/databases/spot/pgs/scores/PGS1/ScoringFiles/PGS1.txt.gz</t>
   </si>
   <si>
@@ -204,7 +222,7 @@
     <t>Australia, Belarus, Belgium, Canada, Denmark, Finland, France, Germany, Greece, Ireland, Netherlands, Norway, Poland, Sweden, UK, USA</t>
   </si>
   <si>
-    <t>ABC, DEF, GHIJ</t>
+    <t>ABC|DEF|GHIJ</t>
   </si>
   <si>
     <t>iCOGS</t>
@@ -650,13 +668,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,31 +723,40 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -738,27 +765,36 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L2">
         <v>10000001</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>26</v>
+      <c r="O2" t="s">
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="R2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -774,13 +810,13 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -789,10 +825,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>11</v>
@@ -801,51 +837,51 @@
         <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H2">
         <v>10000001</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -863,63 +899,63 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>61055</v>
@@ -931,19 +967,19 @@
         <v>30382</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -964,78 +1000,78 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>1234</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1053,51 +1089,51 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>10000001</v>
@@ -1118,30 +1154,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the cohort spreadsheet
</commit_message>
<xml_diff>
--- a/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
+++ b/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
@@ -7,19 +7,89 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Scores" sheetId="1" r:id="rId1"/>
-    <sheet name="Performance Metrics" sheetId="2" r:id="rId2"/>
-    <sheet name="Evaluation Sample Sets" sheetId="3" r:id="rId3"/>
-    <sheet name="Score Development Samples" sheetId="4" r:id="rId4"/>
-    <sheet name="Publications" sheetId="5" r:id="rId5"/>
-    <sheet name="EFO Traits" sheetId="6" r:id="rId6"/>
+    <sheet name="Publications" sheetId="1" r:id="rId1"/>
+    <sheet name="EFO Traits" sheetId="2" r:id="rId2"/>
+    <sheet name="Scores" sheetId="3" r:id="rId3"/>
+    <sheet name="Cohorts" sheetId="4" r:id="rId4"/>
+    <sheet name="Score Development Samples" sheetId="5" r:id="rId5"/>
+    <sheet name="Performance Metrics" sheetId="6" r:id="rId6"/>
+    <sheet name="Evaluation Sample Sets" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="101">
+  <si>
+    <t>PGS Publication/Study (PGP) ID</t>
+  </si>
+  <si>
+    <t>First Author</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Journal Name</t>
+  </si>
+  <si>
+    <t>Publication Date</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>digital object identifier (doi)</t>
+  </si>
+  <si>
+    <t>PubMed ID (PMID)</t>
+  </si>
+  <si>
+    <t>PGP1</t>
+  </si>
+  <si>
+    <t>First T</t>
+  </si>
+  <si>
+    <t>Test publication 1.</t>
+  </si>
+  <si>
+    <t>Test Journal</t>
+  </si>
+  <si>
+    <t>2020-12-01</t>
+  </si>
+  <si>
+    <t>First T, Other A, Other B</t>
+  </si>
+  <si>
+    <t>10.1010/test/test1</t>
+  </si>
+  <si>
+    <t>Ontology Trait ID</t>
+  </si>
+  <si>
+    <t>Ontology Trait Label</t>
+  </si>
+  <si>
+    <t>Ontology Trait Description</t>
+  </si>
+  <si>
+    <t>Ontology URL</t>
+  </si>
+  <si>
+    <t>EFO_0000305</t>
+  </si>
+  <si>
+    <t>breast carcinoma</t>
+  </si>
+  <si>
+    <t>A carcinoma that arises from epithelial cells of the breast [MONDO: DesignPattern]</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0000305</t>
+  </si>
   <si>
     <t>Polygenic Score (PGS) ID</t>
   </si>
@@ -87,12 +157,6 @@
     <t>Breast Cancer</t>
   </si>
   <si>
-    <t>breast carcinoma</t>
-  </si>
-  <si>
-    <t>EFO_0000305</t>
-  </si>
-  <si>
     <t>SNPs passing genome-wide significance</t>
   </si>
   <si>
@@ -102,12 +166,6 @@
     <t>NR</t>
   </si>
   <si>
-    <t>PGP1</t>
-  </si>
-  <si>
-    <t>10.1010/test/test1</t>
-  </si>
-  <si>
     <t>Multi-ancestry (including European):100</t>
   </si>
   <si>
@@ -123,6 +181,93 @@
     <t>PGS obtained from the Catalog should be cited appropriately, and used in accordance with any licensing restrictions set by the authors. See EBI Terms of Use (https://www.ebi.ac.uk/about/terms-of-use/) for additional details.</t>
   </si>
   <si>
+    <t>Cohort ID</t>
+  </si>
+  <si>
+    <t>Cohort Name</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>GHIJ</t>
+  </si>
+  <si>
+    <t>Cohort ABC</t>
+  </si>
+  <si>
+    <t>Cohort DEF</t>
+  </si>
+  <si>
+    <t>Cohort GHIJ</t>
+  </si>
+  <si>
+    <t>Stage of PGS Development</t>
+  </si>
+  <si>
+    <t>Number of Individuals</t>
+  </si>
+  <si>
+    <t>Number of Cases</t>
+  </si>
+  <si>
+    <t>Number of Controls</t>
+  </si>
+  <si>
+    <t>Percent of Participants Who are Male</t>
+  </si>
+  <si>
+    <t>Sample Age</t>
+  </si>
+  <si>
+    <t>Broad Ancestry Category</t>
+  </si>
+  <si>
+    <t>Ancestry (e.g. French, Chinese)</t>
+  </si>
+  <si>
+    <t>Country of Recruitment</t>
+  </si>
+  <si>
+    <t>Additional Ancestry Description</t>
+  </si>
+  <si>
+    <t>Phenotype Definitions and Methods</t>
+  </si>
+  <si>
+    <t>Followup Time</t>
+  </si>
+  <si>
+    <t>GWAS Catalog Study ID (GCST...)</t>
+  </si>
+  <si>
+    <t>Source PubMed ID (PMID) or doi</t>
+  </si>
+  <si>
+    <t>Cohort(s)</t>
+  </si>
+  <si>
+    <t>Additional Sample/Cohort Information</t>
+  </si>
+  <si>
+    <t>Source of Variant Associations (GWAS)</t>
+  </si>
+  <si>
+    <t>European</t>
+  </si>
+  <si>
+    <t>Finland, Sweden, U.S., Australia, Netherlands, Germany, U.K.</t>
+  </si>
+  <si>
+    <t>GCST1</t>
+  </si>
+  <si>
+    <t>10000011</t>
+  </si>
+  <si>
     <t>PGS Performance Metric (PPM) ID</t>
   </si>
   <si>
@@ -171,54 +316,6 @@
     <t>0.522 [0.519,0.527]</t>
   </si>
   <si>
-    <t>Number of Individuals</t>
-  </si>
-  <si>
-    <t>Number of Cases</t>
-  </si>
-  <si>
-    <t>Number of Controls</t>
-  </si>
-  <si>
-    <t>Percent of Participants Who are Male</t>
-  </si>
-  <si>
-    <t>Sample Age</t>
-  </si>
-  <si>
-    <t>Broad Ancestry Category</t>
-  </si>
-  <si>
-    <t>Ancestry (e.g. French, Chinese)</t>
-  </si>
-  <si>
-    <t>Country of Recruitment</t>
-  </si>
-  <si>
-    <t>Additional Ancestry Description</t>
-  </si>
-  <si>
-    <t>Phenotype Definitions and Methods</t>
-  </si>
-  <si>
-    <t>Followup Time</t>
-  </si>
-  <si>
-    <t>GWAS Catalog Study ID (GCST...)</t>
-  </si>
-  <si>
-    <t>Source PubMed ID (PMID) or doi</t>
-  </si>
-  <si>
-    <t>Cohort(s)</t>
-  </si>
-  <si>
-    <t>Additional Sample/Cohort Information</t>
-  </si>
-  <si>
-    <t>European</t>
-  </si>
-  <si>
     <t>Australia, Belarus, Belgium, Canada, Denmark, Finland, France, Germany, Greece, Ireland, Netherlands, Norway, Poland, Sweden, UK, USA</t>
   </si>
   <si>
@@ -226,78 +323,6 @@
   </si>
   <si>
     <t>iCOGS</t>
-  </si>
-  <si>
-    <t>Stage of PGS Development</t>
-  </si>
-  <si>
-    <t>Source of Variant Associations (GWAS)</t>
-  </si>
-  <si>
-    <t>Finland, Sweden, U.S., Australia, Netherlands, Germany, U.K.</t>
-  </si>
-  <si>
-    <t>GCST1</t>
-  </si>
-  <si>
-    <t>10000011</t>
-  </si>
-  <si>
-    <t>PGS Publication/Study (PGP) ID</t>
-  </si>
-  <si>
-    <t>First Author</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Journal Name</t>
-  </si>
-  <si>
-    <t>Publication Date</t>
-  </si>
-  <si>
-    <t>Authors</t>
-  </si>
-  <si>
-    <t>digital object identifier (doi)</t>
-  </si>
-  <si>
-    <t>PubMed ID (PMID)</t>
-  </si>
-  <si>
-    <t>First T</t>
-  </si>
-  <si>
-    <t>Test publication 1.</t>
-  </si>
-  <si>
-    <t>Test Journal</t>
-  </si>
-  <si>
-    <t>2020-12-01</t>
-  </si>
-  <si>
-    <t>First T, Other A, Other B</t>
-  </si>
-  <si>
-    <t>Ontology Trait ID</t>
-  </si>
-  <si>
-    <t>Ontology Trait Label</t>
-  </si>
-  <si>
-    <t>Ontology Trait Description</t>
-  </si>
-  <si>
-    <t>Ontology URL</t>
-  </si>
-  <si>
-    <t>A carcinoma that arises from epithelial cells of the breast [MONDO: DesignPattern]</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0000305</t>
   </si>
 </sst>
 </file>
@@ -668,95 +693,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>10000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -765,31 +899,31 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="L2">
         <v>10000001</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="S2" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -800,7 +934,144 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -810,78 +1081,78 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="H2">
         <v>10000001</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -889,7 +1160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -899,63 +1170,63 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>61055</v>
@@ -967,223 +1238,22 @@
         <v>30382</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="Q2" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2">
-        <v>1234</v>
-      </c>
-      <c r="H2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2">
-        <v>10000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update tests (changing spreadsheet order)
</commit_message>
<xml_diff>
--- a/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
+++ b/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
@@ -10,10 +10,10 @@
     <sheet name="Publications" sheetId="1" r:id="rId1"/>
     <sheet name="EFO Traits" sheetId="2" r:id="rId2"/>
     <sheet name="Scores" sheetId="3" r:id="rId3"/>
-    <sheet name="Cohorts" sheetId="4" r:id="rId4"/>
-    <sheet name="Score Development Samples" sheetId="5" r:id="rId5"/>
-    <sheet name="Performance Metrics" sheetId="6" r:id="rId6"/>
-    <sheet name="Evaluation Sample Sets" sheetId="7" r:id="rId7"/>
+    <sheet name="Score Development Samples" sheetId="4" r:id="rId4"/>
+    <sheet name="Performance Metrics" sheetId="5" r:id="rId5"/>
+    <sheet name="Evaluation Sample Sets" sheetId="6" r:id="rId6"/>
+    <sheet name="Cohorts" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -181,6 +181,126 @@
     <t>PGS obtained from the Catalog should be cited appropriately, and used in accordance with any licensing restrictions set by the authors. See EBI Terms of Use (https://www.ebi.ac.uk/about/terms-of-use/) for additional details.</t>
   </si>
   <si>
+    <t>Stage of PGS Development</t>
+  </si>
+  <si>
+    <t>Number of Individuals</t>
+  </si>
+  <si>
+    <t>Number of Cases</t>
+  </si>
+  <si>
+    <t>Number of Controls</t>
+  </si>
+  <si>
+    <t>Percent of Participants Who are Male</t>
+  </si>
+  <si>
+    <t>Sample Age</t>
+  </si>
+  <si>
+    <t>Broad Ancestry Category</t>
+  </si>
+  <si>
+    <t>Ancestry (e.g. French, Chinese)</t>
+  </si>
+  <si>
+    <t>Country of Recruitment</t>
+  </si>
+  <si>
+    <t>Additional Ancestry Description</t>
+  </si>
+  <si>
+    <t>Phenotype Definitions and Methods</t>
+  </si>
+  <si>
+    <t>Followup Time</t>
+  </si>
+  <si>
+    <t>GWAS Catalog Study ID (GCST...)</t>
+  </si>
+  <si>
+    <t>Source PubMed ID (PMID) or doi</t>
+  </si>
+  <si>
+    <t>Cohort(s)</t>
+  </si>
+  <si>
+    <t>Additional Sample/Cohort Information</t>
+  </si>
+  <si>
+    <t>Source of Variant Associations (GWAS)</t>
+  </si>
+  <si>
+    <t>European</t>
+  </si>
+  <si>
+    <t>Finland, Sweden, U.S., Australia, Netherlands, Germany, U.K.</t>
+  </si>
+  <si>
+    <t>GCST1</t>
+  </si>
+  <si>
+    <t>10000011</t>
+  </si>
+  <si>
+    <t>PGS Performance Metric (PPM) ID</t>
+  </si>
+  <si>
+    <t>Evaluated Score</t>
+  </si>
+  <si>
+    <t>PGS Sample Set (PSS)</t>
+  </si>
+  <si>
+    <t>Covariates Included in the Model</t>
+  </si>
+  <si>
+    <t>PGS Performance: Other Relevant Information</t>
+  </si>
+  <si>
+    <t>Hazard Ratio (HR)</t>
+  </si>
+  <si>
+    <t>Odds Ratio (OR)</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Area Under the Receiver-Operating Characteristic Curve (AUROC)</t>
+  </si>
+  <si>
+    <t>Corcordance Statistic (C-index)</t>
+  </si>
+  <si>
+    <t>Other Metric(s)</t>
+  </si>
+  <si>
+    <t>PPM1</t>
+  </si>
+  <si>
+    <t>PSS1</t>
+  </si>
+  <si>
+    <t>All breast cancer</t>
+  </si>
+  <si>
+    <t>1.53 [1.5,1.56]</t>
+  </si>
+  <si>
+    <t>0.522 [0.519,0.527]</t>
+  </si>
+  <si>
+    <t>Australia, Belarus, Belgium, Canada, Denmark, Finland, France, Germany, Greece, Ireland, Netherlands, Norway, Poland, Sweden, UK, USA</t>
+  </si>
+  <si>
+    <t>ABC|DEF|GHIJ</t>
+  </si>
+  <si>
+    <t>iCOGS</t>
+  </si>
+  <si>
     <t>Cohort ID</t>
   </si>
   <si>
@@ -203,126 +323,6 @@
   </si>
   <si>
     <t>Cohort GHIJ</t>
-  </si>
-  <si>
-    <t>Stage of PGS Development</t>
-  </si>
-  <si>
-    <t>Number of Individuals</t>
-  </si>
-  <si>
-    <t>Number of Cases</t>
-  </si>
-  <si>
-    <t>Number of Controls</t>
-  </si>
-  <si>
-    <t>Percent of Participants Who are Male</t>
-  </si>
-  <si>
-    <t>Sample Age</t>
-  </si>
-  <si>
-    <t>Broad Ancestry Category</t>
-  </si>
-  <si>
-    <t>Ancestry (e.g. French, Chinese)</t>
-  </si>
-  <si>
-    <t>Country of Recruitment</t>
-  </si>
-  <si>
-    <t>Additional Ancestry Description</t>
-  </si>
-  <si>
-    <t>Phenotype Definitions and Methods</t>
-  </si>
-  <si>
-    <t>Followup Time</t>
-  </si>
-  <si>
-    <t>GWAS Catalog Study ID (GCST...)</t>
-  </si>
-  <si>
-    <t>Source PubMed ID (PMID) or doi</t>
-  </si>
-  <si>
-    <t>Cohort(s)</t>
-  </si>
-  <si>
-    <t>Additional Sample/Cohort Information</t>
-  </si>
-  <si>
-    <t>Source of Variant Associations (GWAS)</t>
-  </si>
-  <si>
-    <t>European</t>
-  </si>
-  <si>
-    <t>Finland, Sweden, U.S., Australia, Netherlands, Germany, U.K.</t>
-  </si>
-  <si>
-    <t>GCST1</t>
-  </si>
-  <si>
-    <t>10000011</t>
-  </si>
-  <si>
-    <t>PGS Performance Metric (PPM) ID</t>
-  </si>
-  <si>
-    <t>Evaluated Score</t>
-  </si>
-  <si>
-    <t>PGS Sample Set (PSS)</t>
-  </si>
-  <si>
-    <t>Covariates Included in the Model</t>
-  </si>
-  <si>
-    <t>PGS Performance: Other Relevant Information</t>
-  </si>
-  <si>
-    <t>Hazard Ratio (HR)</t>
-  </si>
-  <si>
-    <t>Odds Ratio (OR)</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>Area Under the Receiver-Operating Characteristic Curve (AUROC)</t>
-  </si>
-  <si>
-    <t>Corcordance Statistic (C-index)</t>
-  </si>
-  <si>
-    <t>Other Metric(s)</t>
-  </si>
-  <si>
-    <t>PPM1</t>
-  </si>
-  <si>
-    <t>PSS1</t>
-  </si>
-  <si>
-    <t>All breast cancer</t>
-  </si>
-  <si>
-    <t>1.53 [1.5,1.56]</t>
-  </si>
-  <si>
-    <t>0.522 [0.519,0.527]</t>
-  </si>
-  <si>
-    <t>Australia, Belarus, Belgium, Canada, Denmark, Finland, France, Germany, Greece, Ireland, Netherlands, Norway, Poland, Sweden, UK, USA</t>
-  </si>
-  <si>
-    <t>ABC|DEF|GHIJ</t>
-  </si>
-  <si>
-    <t>iCOGS</t>
   </si>
 </sst>
 </file>
@@ -936,42 +936,89 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -980,6 +1027,95 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2">
+        <v>10000001</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -989,170 +1125,87 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2">
-        <v>1234</v>
-      </c>
-      <c r="H2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" t="s">
-        <v>80</v>
-      </c>
-      <c r="O2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2">
-        <v>10000001</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" t="s">
-        <v>97</v>
+      <c r="C2">
+        <v>61055</v>
+      </c>
+      <c r="D2">
+        <v>30673</v>
+      </c>
+      <c r="E2">
+        <v>30382</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1162,94 +1215,41 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2">
-        <v>61055</v>
-      </c>
-      <c r="D2">
-        <v>30673</v>
-      </c>
-      <c r="E2">
-        <v>30382</v>
-      </c>
-      <c r="H2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" t="s">
         <v>98</v>
       </c>
-      <c r="L2" t="s">
-        <v>95</v>
-      </c>
-      <c r="P2" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
         <v>99</v>
       </c>
-      <c r="Q2" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Split the PMID column in PMID and DOI columns (sample and performance)
</commit_message>
<xml_diff>
--- a/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
+++ b/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
   <si>
     <t>PGS Publication/Study (PGP) ID</t>
   </si>
@@ -220,7 +220,10 @@
     <t>GWAS Catalog Study ID (GCST...)</t>
   </si>
   <si>
-    <t>Source PubMed ID (PMID) or doi</t>
+    <t>Source PubMed ID (PMID)</t>
+  </si>
+  <si>
+    <t>Source DOI</t>
   </si>
   <si>
     <t>Cohort(s)</t>
@@ -241,9 +244,6 @@
     <t>GCST1</t>
   </si>
   <si>
-    <t>10000011</t>
-  </si>
-  <si>
     <t>PGS Performance Metric (PPM) ID</t>
   </si>
   <si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>Australia, Belarus, Belgium, Canada, Denmark, Finland, France, Germany, Greece, Ireland, Netherlands, Norway, Poland, Sweden, UK, USA</t>
+  </si>
+  <si>
+    <t>10.2021/pgs.1001</t>
   </si>
   <si>
     <t>ABC|DEF|GHIJ</t>
@@ -936,13 +939,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -994,31 +997,34 @@
       <c r="Q1" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>1234</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
         <v>47</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" t="s">
         <v>73</v>
+      </c>
+      <c r="O2">
+        <v>10000011</v>
       </c>
     </row>
   </sheetData>
@@ -1117,13 +1123,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -1175,8 +1181,11 @@
       <c r="Q1" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1193,7 +1202,7 @@
         <v>30382</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
         <v>90</v>
@@ -1206,6 +1215,9 @@
       </c>
       <c r="Q2" t="s">
         <v>92</v>
+      </c>
+      <c r="R2" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1223,34 +1235,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add export for large publications + started to add weight_type (for Scores).
</commit_message>
<xml_diff>
--- a/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
+++ b/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t>PGS Publication/Study (PGP) ID</t>
   </si>
@@ -121,6 +121,9 @@
     <t>Number of Interaction Terms</t>
   </si>
   <si>
+    <t>Type of Variant Weight</t>
+  </si>
+  <si>
     <t>PGS Publication (PGP) ID</t>
   </si>
   <si>
@@ -164,6 +167,9 @@
   </si>
   <si>
     <t>NR</t>
+  </si>
+  <si>
+    <t>log(OR)</t>
   </si>
   <si>
     <t>Multi-ancestry (including European):100</t>
@@ -805,13 +811,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -869,16 +875,19 @@
       <c r="S1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -887,13 +896,13 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -902,36 +911,39 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>10000001</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" t="b">
+      <c r="O2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
-        <v>48</v>
-      </c>
       <c r="P2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="S2" t="s">
+      <c r="R2" t="s">
         <v>52</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1"/>
+    <hyperlink ref="S2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -950,78 +962,78 @@
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>1234</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O2">
         <v>10000011</v>
@@ -1042,66 +1054,66 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H2">
         <v>10000001</v>
@@ -1110,10 +1122,10 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="N2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1131,66 +1143,66 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>61055</v>
@@ -1202,22 +1214,22 @@
         <v>30382</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="P2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="Q2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="R2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1235,34 +1247,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new Cohort field 'name_others'
</commit_message>
<xml_diff>
--- a/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
+++ b/tests/output/PGS1/Metadata/PGS1_metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
   <si>
     <t>PGS Publication/Study (PGP) ID</t>
   </si>
@@ -316,6 +316,9 @@
     <t>Cohort Name</t>
   </si>
   <si>
+    <t>Previous/other/additional names</t>
+  </si>
+  <si>
     <t>ABC</t>
   </si>
   <si>
@@ -332,6 +335,9 @@
   </si>
   <si>
     <t>Cohort GHIJ</t>
+  </si>
+  <si>
+    <t>ABC-1</t>
   </si>
 </sst>
 </file>
@@ -1239,42 +1245,48 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>100</v>
-      </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>